<commit_message>
Rate and My Agenda Test Cases added
</commit_message>
<xml_diff>
--- a/Test Data/TestData.xlsx
+++ b/Test Data/TestData.xlsx
@@ -55,13 +55,13 @@
     <t xml:space="preserve">https://web.event2mobile.com/</t>
   </si>
   <si>
-    <t xml:space="preserve">/Browser_Driver/geckodriver</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/Browser_Driver/chromedriver</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/Browser_Driver/firefoxLogs</t>
+    <t xml:space="preserve">/Browser Driver/geckodriver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Browser Driver/chromedriver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Browser Driver/firefoxLogs</t>
   </si>
   <si>
     <t xml:space="preserve">brucewills@yopmail.com</t>
@@ -124,6 +124,7 @@
       <color rgb="FF2A00FF"/>
       <name val="Monaco"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -298,20 +299,20 @@
   </sheetPr>
   <dimension ref="A1:AMJ2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="28.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="26.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="25.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="25.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="34.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="34.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="42.01"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="11.52"/>
   </cols>

</xml_diff>